<commit_message>
Solved Problem List with Hint. (UPDATED Nov-25-2019)
</commit_message>
<xml_diff>
--- a/Problem_List.xlsx
+++ b/Problem_List.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ComputerScience\C++ Codes\lgnew\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C695BC67-6DFA-424F-B144-379FDA3C61A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{705DAD80-3ADC-48CD-962D-FC53F789DD6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{DE3CDA67-778D-4607-BB5A-3AF7AE70AB80}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="148">
   <si>
     <t>P1000</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -898,6 +898,26 @@
       <t>统计每个区间，若两个区间可以“套起来”（区间的左端在当前段的右端内）就合并作一个区间（设右端为新区间的右端），否则视作一个区间结束，累计长度，加起来就是应砍掉树的数目。
 （当然根据这题的数据量也可以模拟水过）</t>
     </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P1088</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>火星人</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数学</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>使用STL算法next_permutation可以水过</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1393,10 +1413,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B67F7112-CDED-4A6B-89D1-B41CC13758BD}">
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2172,6 +2192,32 @@
         <v>43750</v>
       </c>
     </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>143</v>
+      </c>
+      <c r="B31" t="s">
+        <v>144</v>
+      </c>
+      <c r="C31" t="s">
+        <v>145</v>
+      </c>
+      <c r="D31" t="s">
+        <v>66</v>
+      </c>
+      <c r="E31" t="s">
+        <v>146</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="G31" s="4">
+        <v>43794</v>
+      </c>
+      <c r="H31" s="4">
+        <v>43794</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:H15" xr:uid="{880B8996-DDC7-47AA-9C04-AA5D01911FE9}"/>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
UPDATED 12/30/2019: P1219 Solved
</commit_message>
<xml_diff>
--- a/Problem_List.xlsx
+++ b/Problem_List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ComputerScience\C++ Codes\lgnew\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{705DAD80-3ADC-48CD-962D-FC53F789DD6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E78C45A-DE5D-4A57-BBF1-7CF11F033892}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{DE3CDA67-778D-4607-BB5A-3AF7AE70AB80}"/>
+    <workbookView xWindow="7524" yWindow="1896" windowWidth="11040" windowHeight="10464" xr2:uid="{DE3CDA67-778D-4607-BB5A-3AF7AE70AB80}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="165">
   <si>
     <t>P1000</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -920,12 +920,92 @@
     <t>使用STL算法next_permutation可以水过</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>P1605</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>迷宫</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>普及-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DFS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>基本的DFS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P1601</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A+B Problem（高精度版）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>普及-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>高精度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>高精度加法模板</t>
+  </si>
+  <si>
+    <t>P1219</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>八皇后</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DFS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">逐行处理（每行一层递归），检查该行中有无格未被占用，然后把该格序号填入，退出递归时撤销序号
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0" tint="-0.249977111117893"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>（PS：最后一个点n=13谜之超时，只能打表过？）</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1010,6 +1090,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF00B050"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.249977111117893"/>
       <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
@@ -1413,10 +1501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B67F7112-CDED-4A6B-89D1-B41CC13758BD}">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="F39" sqref="F38:F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2218,6 +2306,84 @@
         <v>43794</v>
       </c>
     </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>148</v>
+      </c>
+      <c r="B32" t="s">
+        <v>149</v>
+      </c>
+      <c r="C32" t="s">
+        <v>150</v>
+      </c>
+      <c r="D32" t="s">
+        <v>151</v>
+      </c>
+      <c r="E32" t="s">
+        <v>152</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="G32" s="4">
+        <v>43817</v>
+      </c>
+      <c r="H32" s="4">
+        <v>43817</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>154</v>
+      </c>
+      <c r="B33" t="s">
+        <v>155</v>
+      </c>
+      <c r="C33" t="s">
+        <v>156</v>
+      </c>
+      <c r="D33" t="s">
+        <v>157</v>
+      </c>
+      <c r="E33" t="s">
+        <v>158</v>
+      </c>
+      <c r="F33" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="G33" s="4">
+        <v>43818</v>
+      </c>
+      <c r="H33" s="4">
+        <v>43818</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>160</v>
+      </c>
+      <c r="B34" t="s">
+        <v>161</v>
+      </c>
+      <c r="C34" t="s">
+        <v>162</v>
+      </c>
+      <c r="D34" t="s">
+        <v>66</v>
+      </c>
+      <c r="E34" t="s">
+        <v>163</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="G34" s="4">
+        <v>43807</v>
+      </c>
+      <c r="H34" s="4">
+        <v>43829</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:H15" xr:uid="{880B8996-DDC7-47AA-9C04-AA5D01911FE9}"/>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Test GitHub Commit - 2020/8/3
</commit_message>
<xml_diff>
--- a/Problem_List.xlsx
+++ b/Problem_List.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ComputerScience\C++ Codes\lgnew\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E78C45A-DE5D-4A57-BBF1-7CF11F033892}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{622C479E-FE2A-40CA-BFB1-F0250909D542}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7524" yWindow="1896" windowWidth="11040" windowHeight="10464" xr2:uid="{DE3CDA67-778D-4607-BB5A-3AF7AE70AB80}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{DE3CDA67-778D-4607-BB5A-3AF7AE70AB80}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$15</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$43</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="278">
   <si>
     <t>P1000</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -249,31 +249,6 @@
   </si>
   <si>
     <t>机器翻译</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>搜索/暴力</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DP/递推</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>搜索/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFFC000"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>状态压缩</t>
-    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -365,10 +340,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>搜索/记忆化</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>无他，唯模拟尔
 注意胜负表的对称（斯波克对蜥蜴人负，就要记得添上蜥蜴人对斯波克胜）</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -450,10 +421,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>HINT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>注意移牌只能在相邻堆之间进行。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -467,10 +434,6 @@
   </si>
   <si>
     <t>花生采摘</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>模拟+贪心</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -521,10 +484,6 @@
   </si>
   <si>
     <t>魔法照片</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>模拟+排序</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -770,10 +729,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>计算</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>在建立明文-&gt;密文的表时，可以再建立一个密文-&gt;明文的表</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -917,10 +872,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>使用STL算法next_permutation可以水过</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>P1605</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -985,7 +936,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">逐行处理（每行一层递归），检查该行中有无格未被占用，然后把该格序号填入，退出递归时撤销序号
+      <t xml:space="preserve">逐行处理（每行一层递归），检查该行中有无格未被占用，然后把该格序号填入排行表，退出递归时撤销序号
 </t>
     </r>
     <r>
@@ -999,13 +950,623 @@
       </rPr>
       <t>（PS：最后一个点n=13谜之超时，只能打表过？）</t>
     </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P1075</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>质因数分解</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>入门</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数学</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用筛法制表，从最小的质数找起，找到因子就做n/primes[i]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P1076</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>寻宝</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P5461</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>赦免战俘</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>分治</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>分治思路较为清晰，按题目描述操作
+以最初的方阵中心点(2^(n-1),2^(n-1))开始，将中心点左上（包括该点）全部清零，再递归地去找下三个中心点</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P1010</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>幂次方</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>普及-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>分治</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>对一个数x，每次都取不大于它的最大2的幂，对指数再继续分解，注意1、2、3的处理</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>数学/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>STL</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">使用STL算法next_permutation可以水过
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0" tint="-0.249977111117893"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>（</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0" tint="-0.249977111117893"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>PS：NOIP2003时还不允许用STL，因此需要手写next_permutation，难度较高，故它被排在第三题）</t>
+    </r>
+  </si>
+  <si>
+    <t>P1009</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>阶乘之和</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>高精度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>高精度加法+乘法</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P4924</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>普及-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>模拟</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>魔法少女小Scarlet</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>普及/提高-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>注意顺、逆时针旋转的实质（顺时针=转置+左右翻转，逆时针=转置+上下翻转）和相对坐标</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P1518</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>两只塔姆沃斯牛</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P1060</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>开心的金明</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>01背包变种。花费为v[i]，价值为v[i]*w[i]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P1049</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>装箱问题</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>01背包变种。花费和价值均为w[i]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HINT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>注意重复状态的判断（同时描述FJ和牛的位置和各自方向，若有重复则说明循环，不会相遇）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P1065</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>作业调度方案</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>模拟</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HALTED</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P1591</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>阶乘数码</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>普及-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>高精度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>高精度乘法</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P1045</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>麦森数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P2676</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>超级书架</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>入门</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>排序</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>先选最大的牛</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P1116</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>车厢重组</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>对于只交换相邻元素的排序，最少需要进行的操作数等于每一个元素前比它大的元素数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P1152</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>欢乐的跳</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>将每两个元素的差构成的数组排序，判断其是否是公差为1的递增等差数列</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P5143</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>攀爬者</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>按高度递增排序</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P2089</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>烤鸡</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P2241</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>统计方形</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>枚举</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>对于每个格点(x,y)，以其为顶点的正方形共有min(x,y)+min(n-x,m-y)+min(m-y,x)+min(y,n-x)个，矩形数为n*m-(正方形数)。又因为每个正方形会被重复算4次，故输出时/4。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>对10种调料做10层循环枚举</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P3392</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>涂国旗</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>枚举</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P3654</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>First Step</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>普及-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>对每一个空格，分别向下、向右判断其是否能拓展到k格</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P1149</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>火柴棒等式</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>普及-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>枚举</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P3799</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>妖梦拼木棒</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>枚举0~999范围内的数，判断这些数及其和数所用火柴棒数是否等于(n-4)。注意i、j、i+j位数不同时的处理</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>先统计每种长度木棒的数目，若有一种长度有至少2根木棒，再检查比它短的木棒里有无能凑成和它一样长的，答案为
+Σ(C(count[i],2)*count[j]*count[i-j])（凑成i的木棒不一样长的)
++Σ(C(count[i],2)*C(count[j],2)) （凑成i的木棒一样长的）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>高精度减法+乘法，2^p的位数可以用公式q=floor(plg2)+1来计算。注意最大需要处理2^1000000，直接乘2很慢，可以用每次乘2^15加速</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P1255</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数楼梯</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P1044</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>栈</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>假设第i个元素的出栈顺序一共有h[i]种。需要注意的是</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1~n每个元素都可能是最后一个出栈的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>。易证本问题有</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>最优子结构</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">性质。对于第k个元素，在它之前入栈、之前出栈的有k-1个元素，出栈顺序有h[k-1]种；在它之后入栈、之前出栈的有n-k个元素，出栈顺序有h[n-k]种，故
+h[k]=Σ(h[k-1]*h[n-k])
+</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P1028</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数的计算</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>f[i]=f[1]+f[2]+…+f[i/2],1&lt;=i&lt;=n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P1928</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>外星密码</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>普及+/提高</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>分治</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P2437</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>蜜蜂路线</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>普及-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>字符串处理+排序</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>搜索(记忆化搜索)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>搜索(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>状态压缩</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>DP(背包)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DP(递推)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>模拟+贪心</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>高精斐波那契数列</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P1164</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>小A点菜</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>搜索(DFS)/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DP</t>
+    </r>
+  </si>
+  <si>
+    <t>每个状态记录当前进行到第几道菜以及目前所花的钱数。对于每个状态，都拓展出吃和不吃两个子状态，注意剪枝</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1103,8 +1664,47 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.249977111117893"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1126,8 +1726,32 @@
         <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -1135,8 +1759,53 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right style="thick">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="thick">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFF33CC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFFF33CC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFFF33CC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFFF33CC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF00B050"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF00B050"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF00B050"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF00B050"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1149,8 +1818,11 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1175,17 +1847,36 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="3">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="3" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="4">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="4" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
+    <cellStyle name="40% - 着色 3" xfId="4" builtinId="39"/>
     <cellStyle name="差" xfId="3" builtinId="27"/>
     <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="好" xfId="1" builtinId="26"/>
@@ -1193,6 +1884,12 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF00FFFF"/>
+      <color rgb="FFFF33CC"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1501,10 +2198,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B67F7112-CDED-4A6B-89D1-B41CC13758BD}">
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:H62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="F39" sqref="F38:F39"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="A63" sqref="A63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1512,8 +2209,8 @@
     <col min="1" max="1" width="11.21875" customWidth="1"/>
     <col min="2" max="2" width="32" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="13.5546875" customWidth="1"/>
-    <col min="6" max="6" width="56.5546875" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" customWidth="1"/>
+    <col min="6" max="6" width="56.5546875" style="2" customWidth="1"/>
     <col min="7" max="7" width="11.21875" customWidth="1"/>
     <col min="8" max="8" width="11.21875" bestFit="1" customWidth="1"/>
   </cols>
@@ -1534,7 +2231,7 @@
       <c r="E1" t="s">
         <v>14</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="G1" t="s">
@@ -1558,9 +2255,9 @@
         <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>110</v>
-      </c>
-      <c r="F2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>10</v>
       </c>
       <c r="G2" s="4">
@@ -1586,7 +2283,7 @@
       <c r="E3" t="s">
         <v>15</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="2" t="s">
         <v>15</v>
       </c>
       <c r="G3" s="4">
@@ -1610,10 +2307,10 @@
         <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>42</v>
+        <v>271</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="G4" s="4">
         <v>43713</v>
@@ -1636,7 +2333,7 @@
         <v>13</v>
       </c>
       <c r="E5" t="s">
-        <v>43</v>
+        <v>269</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>20</v>
@@ -1714,7 +2411,7 @@
         <v>33</v>
       </c>
       <c r="E8" t="s">
-        <v>41</v>
+        <v>228</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>34</v>
@@ -1730,7 +2427,7 @@
       <c r="A9" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="15" t="s">
         <v>36</v>
       </c>
       <c r="C9" t="s">
@@ -1740,10 +2437,10 @@
         <v>13</v>
       </c>
       <c r="E9" t="s">
-        <v>41</v>
+        <v>228</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="G9" s="4">
         <v>43716</v>
@@ -1769,7 +2466,7 @@
         <v>27</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="G10" s="4">
         <v>43716</v>
@@ -1780,22 +2477,22 @@
     </row>
     <row r="11" spans="1:8" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" t="s">
         <v>44</v>
       </c>
-      <c r="B11" t="s">
-        <v>45</v>
-      </c>
-      <c r="C11" t="s">
-        <v>48</v>
-      </c>
-      <c r="D11" t="s">
-        <v>46</v>
-      </c>
-      <c r="E11" t="s">
-        <v>47</v>
-      </c>
       <c r="F11" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="G11" s="4">
         <v>43718</v>
@@ -1806,22 +2503,22 @@
     </row>
     <row r="12" spans="1:8" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" t="s">
         <v>49</v>
       </c>
-      <c r="B12" t="s">
-        <v>50</v>
-      </c>
-      <c r="C12" t="s">
-        <v>53</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="F12" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="E12" t="s">
-        <v>52</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>54</v>
       </c>
       <c r="G12" s="4">
         <v>43719</v>
@@ -1832,22 +2529,22 @@
     </row>
     <row r="13" spans="1:8" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" t="s">
         <v>55</v>
       </c>
-      <c r="B13" t="s">
+      <c r="E13" t="s">
+        <v>138</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="C13" t="s">
-        <v>57</v>
-      </c>
-      <c r="D13" t="s">
-        <v>58</v>
-      </c>
-      <c r="E13" t="s">
-        <v>114</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>59</v>
       </c>
       <c r="G13" s="4">
         <v>43724</v>
@@ -1858,10 +2555,10 @@
     </row>
     <row r="14" spans="1:8" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B14" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C14" t="s">
         <v>5</v>
@@ -1870,10 +2567,10 @@
         <v>13</v>
       </c>
       <c r="E14" t="s">
-        <v>62</v>
+        <v>268</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="G14" s="4">
         <v>43724</v>
@@ -1883,40 +2580,40 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
-        <v>64</v>
+      <c r="A15" s="10" t="s">
+        <v>60</v>
       </c>
       <c r="B15" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C15" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="D15" t="s">
+        <v>62</v>
+      </c>
+      <c r="E15" t="s">
         <v>66</v>
-      </c>
-      <c r="E15" t="s">
-        <v>70</v>
       </c>
       <c r="G15" s="4">
         <v>43728</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>67</v>
+      <c r="A16" s="10" t="s">
+        <v>63</v>
       </c>
       <c r="B16" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C16" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D16" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E16" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="G16" s="4">
         <v>43731</v>
@@ -1924,22 +2621,22 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" t="s">
+        <v>68</v>
+      </c>
+      <c r="C17" t="s">
+        <v>70</v>
+      </c>
+      <c r="D17" t="s">
+        <v>69</v>
+      </c>
+      <c r="E17" t="s">
+        <v>66</v>
+      </c>
+      <c r="F17" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="B17" t="s">
-        <v>72</v>
-      </c>
-      <c r="C17" t="s">
-        <v>74</v>
-      </c>
-      <c r="D17" t="s">
-        <v>73</v>
-      </c>
-      <c r="E17" t="s">
-        <v>70</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>75</v>
       </c>
       <c r="G17" s="4">
         <v>43732</v>
@@ -1949,23 +2646,23 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="B18" t="s">
+        <v>73</v>
+      </c>
+      <c r="C18" t="s">
         <v>76</v>
       </c>
-      <c r="B18" t="s">
-        <v>77</v>
-      </c>
-      <c r="C18" t="s">
-        <v>83</v>
-      </c>
       <c r="D18" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E18" t="s">
+        <v>75</v>
+      </c>
+      <c r="F18" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>84</v>
       </c>
       <c r="G18" s="4">
         <v>43732</v>
@@ -1973,22 +2670,22 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B19" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C19" t="s">
         <v>5</v>
       </c>
       <c r="D19" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E19" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="G19" s="4">
         <v>43732</v>
@@ -1999,22 +2696,22 @@
     </row>
     <row r="20" spans="1:8" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B20" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C20" t="s">
         <v>5</v>
       </c>
       <c r="D20" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E20" t="s">
-        <v>88</v>
+        <v>272</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="G20" s="4">
         <v>43734</v>
@@ -2025,22 +2722,22 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B21" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C21" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="D21" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="E21" t="s">
-        <v>93</v>
-      </c>
-      <c r="F21" s="9" t="s">
-        <v>94</v>
+        <v>87</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>88</v>
       </c>
       <c r="G21" s="4">
         <v>43739</v>
@@ -2051,22 +2748,22 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B22" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C22" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="D22" t="s">
+        <v>86</v>
+      </c>
+      <c r="E22" t="s">
+        <v>213</v>
+      </c>
+      <c r="F22" s="2" t="s">
         <v>92</v>
-      </c>
-      <c r="E22" t="s">
-        <v>98</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>99</v>
       </c>
       <c r="G22" s="4">
         <v>43739</v>
@@ -2077,22 +2774,22 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="B23" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="C23" t="s">
+        <v>89</v>
+      </c>
+      <c r="D23" t="s">
+        <v>86</v>
+      </c>
+      <c r="E23" t="s">
+        <v>213</v>
+      </c>
+      <c r="F23" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="D23" t="s">
-        <v>92</v>
-      </c>
-      <c r="E23" t="s">
-        <v>98</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>102</v>
       </c>
       <c r="G23" s="4">
         <v>43740</v>
@@ -2103,22 +2800,22 @@
     </row>
     <row r="24" spans="1:8" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="B24" t="s">
+        <v>97</v>
+      </c>
+      <c r="C24" t="s">
+        <v>89</v>
+      </c>
+      <c r="D24" t="s">
+        <v>86</v>
+      </c>
+      <c r="E24" t="s">
+        <v>98</v>
+      </c>
+      <c r="F24" s="8" t="s">
         <v>104</v>
-      </c>
-      <c r="C24" t="s">
-        <v>95</v>
-      </c>
-      <c r="D24" t="s">
-        <v>92</v>
-      </c>
-      <c r="E24" t="s">
-        <v>105</v>
-      </c>
-      <c r="F24" s="10" t="s">
-        <v>111</v>
       </c>
       <c r="G24" s="4">
         <v>43740</v>
@@ -2129,22 +2826,22 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="B25" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="C25" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="D25" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E25" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="G25" s="4">
         <v>43741</v>
@@ -2155,22 +2852,22 @@
     </row>
     <row r="26" spans="1:8" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="B26" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="C26" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="D26" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="E26" t="s">
-        <v>105</v>
+        <v>267</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="G26" s="4">
         <v>43741</v>
@@ -2181,22 +2878,22 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="B27" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="C27" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="D27" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E27" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="G27" s="4">
         <v>43741</v>
@@ -2204,22 +2901,22 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="B28" t="s">
+        <v>119</v>
+      </c>
+      <c r="C28" t="s">
+        <v>120</v>
+      </c>
+      <c r="D28" t="s">
+        <v>121</v>
+      </c>
+      <c r="E28" t="s">
+        <v>122</v>
+      </c>
+      <c r="F28" s="2" t="s">
         <v>127</v>
-      </c>
-      <c r="C28" t="s">
-        <v>128</v>
-      </c>
-      <c r="D28" t="s">
-        <v>129</v>
-      </c>
-      <c r="E28" t="s">
-        <v>130</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>135</v>
       </c>
       <c r="G28" s="4">
         <v>43746</v>
@@ -2230,22 +2927,22 @@
     </row>
     <row r="29" spans="1:8" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="B29" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C29" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="D29" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="E29" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="G29" s="4">
         <v>43747</v>
@@ -2256,22 +2953,22 @@
     </row>
     <row r="30" spans="1:8" ht="82.8" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="B30" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="C30" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="D30" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="E30" t="s">
-        <v>141</v>
-      </c>
-      <c r="F30" s="10" t="s">
-        <v>142</v>
+        <v>133</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>134</v>
       </c>
       <c r="G30" s="4">
         <v>43750</v>
@@ -2280,24 +2977,24 @@
         <v>43750</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="B31" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="C31" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="D31" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E31" t="s">
-        <v>146</v>
+        <v>175</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>147</v>
+        <v>176</v>
       </c>
       <c r="G31" s="4">
         <v>43794</v>
@@ -2308,22 +3005,22 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="B32" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="C32" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="D32" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="E32" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="G32" s="4">
         <v>43817</v>
@@ -2334,22 +3031,22 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="B33" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="C33" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="D33" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="E33" t="s">
-        <v>158</v>
-      </c>
-      <c r="F33" s="9" t="s">
-        <v>159</v>
+        <v>149</v>
+      </c>
+      <c r="F33" s="8" t="s">
+        <v>150</v>
       </c>
       <c r="G33" s="4">
         <v>43818</v>
@@ -2360,22 +3057,22 @@
     </row>
     <row r="34" spans="1:8" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="B34" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="C34" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="D34" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E34" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="G34" s="4">
         <v>43807</v>
@@ -2384,8 +3081,709 @@
         <v>43829</v>
       </c>
     </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>156</v>
+      </c>
+      <c r="B35" t="s">
+        <v>157</v>
+      </c>
+      <c r="C35" t="s">
+        <v>158</v>
+      </c>
+      <c r="D35" t="s">
+        <v>159</v>
+      </c>
+      <c r="E35" t="s">
+        <v>160</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="G35" s="4">
+        <v>43829</v>
+      </c>
+      <c r="H35" s="4">
+        <v>43831</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>162</v>
+      </c>
+      <c r="B36" t="s">
+        <v>163</v>
+      </c>
+      <c r="C36" t="s">
+        <v>76</v>
+      </c>
+      <c r="D36" t="s">
+        <v>62</v>
+      </c>
+      <c r="E36" t="s">
+        <v>184</v>
+      </c>
+      <c r="G36" s="4">
+        <v>43831</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="B37" t="s">
+        <v>165</v>
+      </c>
+      <c r="C37" t="s">
+        <v>166</v>
+      </c>
+      <c r="D37" t="s">
+        <v>62</v>
+      </c>
+      <c r="E37" t="s">
+        <v>167</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="G37" s="4">
+        <v>43865</v>
+      </c>
+      <c r="H37" s="4">
+        <v>43866</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>169</v>
+      </c>
+      <c r="B38" t="s">
+        <v>170</v>
+      </c>
+      <c r="C38" t="s">
+        <v>171</v>
+      </c>
+      <c r="D38" t="s">
+        <v>172</v>
+      </c>
+      <c r="E38" t="s">
+        <v>173</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="G38" s="4">
+        <v>43867</v>
+      </c>
+      <c r="H38" s="4">
+        <v>43867</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>190</v>
+      </c>
+      <c r="B39" t="s">
+        <v>191</v>
+      </c>
+      <c r="C39" t="s">
+        <v>179</v>
+      </c>
+      <c r="D39" t="s">
+        <v>183</v>
+      </c>
+      <c r="E39" t="s">
+        <v>270</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="G39" s="4">
+        <v>43910</v>
+      </c>
+      <c r="H39" s="4">
+        <v>43910</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>193</v>
+      </c>
+      <c r="B40" t="s">
+        <v>194</v>
+      </c>
+      <c r="C40" t="s">
+        <v>179</v>
+      </c>
+      <c r="D40" t="s">
+        <v>183</v>
+      </c>
+      <c r="E40" t="s">
+        <v>270</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="G40" s="4">
+        <v>43910</v>
+      </c>
+      <c r="H40" s="4">
+        <v>43910</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>177</v>
+      </c>
+      <c r="B41" t="s">
+        <v>178</v>
+      </c>
+      <c r="C41" t="s">
+        <v>179</v>
+      </c>
+      <c r="D41" t="s">
+        <v>183</v>
+      </c>
+      <c r="E41" t="s">
+        <v>180</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="G41" s="4">
+        <v>43920</v>
+      </c>
+      <c r="H41" s="4">
+        <v>43920</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="28.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>182</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="C42" t="s">
+        <v>179</v>
+      </c>
+      <c r="D42" t="s">
+        <v>186</v>
+      </c>
+      <c r="E42" t="s">
+        <v>184</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="G42" s="4">
+        <v>43920</v>
+      </c>
+      <c r="H42" s="4">
+        <v>43921</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="28.2" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="B43" t="s">
+        <v>189</v>
+      </c>
+      <c r="C43" t="s">
+        <v>196</v>
+      </c>
+      <c r="D43" t="s">
+        <v>62</v>
+      </c>
+      <c r="E43" t="s">
+        <v>184</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="G43" s="4">
+        <v>43921</v>
+      </c>
+      <c r="H43" s="4">
+        <v>43922</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="B44" t="s">
+        <v>199</v>
+      </c>
+      <c r="C44" t="s">
+        <v>201</v>
+      </c>
+      <c r="D44" t="s">
+        <v>62</v>
+      </c>
+      <c r="E44" t="s">
+        <v>200</v>
+      </c>
+      <c r="G44" s="4">
+        <v>43923</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>202</v>
+      </c>
+      <c r="B45" t="s">
+        <v>203</v>
+      </c>
+      <c r="C45" t="s">
+        <v>204</v>
+      </c>
+      <c r="D45" t="s">
+        <v>205</v>
+      </c>
+      <c r="E45" t="s">
+        <v>206</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="G45" s="4">
+        <v>43927</v>
+      </c>
+      <c r="H45" s="4">
+        <v>43927</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>208</v>
+      </c>
+      <c r="B46" t="s">
+        <v>209</v>
+      </c>
+      <c r="C46" t="s">
+        <v>204</v>
+      </c>
+      <c r="D46" t="s">
+        <v>62</v>
+      </c>
+      <c r="E46" t="s">
+        <v>206</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="G46" s="4">
+        <v>43927</v>
+      </c>
+      <c r="H46" s="4">
+        <v>43927</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>210</v>
+      </c>
+      <c r="B47" t="s">
+        <v>211</v>
+      </c>
+      <c r="C47" t="s">
+        <v>204</v>
+      </c>
+      <c r="D47" t="s">
+        <v>212</v>
+      </c>
+      <c r="E47" t="s">
+        <v>213</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="G47" s="4">
+        <v>43927</v>
+      </c>
+      <c r="H47" s="4">
+        <v>43927</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>215</v>
+      </c>
+      <c r="B48" t="s">
+        <v>216</v>
+      </c>
+      <c r="C48" t="s">
+        <v>204</v>
+      </c>
+      <c r="D48" t="s">
+        <v>212</v>
+      </c>
+      <c r="E48" t="s">
+        <v>213</v>
+      </c>
+      <c r="F48" s="12" t="s">
+        <v>217</v>
+      </c>
+      <c r="G48" s="4">
+        <v>43927</v>
+      </c>
+      <c r="H48" s="4">
+        <v>43927</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>218</v>
+      </c>
+      <c r="B49" t="s">
+        <v>219</v>
+      </c>
+      <c r="C49" t="s">
+        <v>204</v>
+      </c>
+      <c r="D49" t="s">
+        <v>212</v>
+      </c>
+      <c r="E49" t="s">
+        <v>213</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="G49" s="4">
+        <v>43927</v>
+      </c>
+      <c r="H49" s="4">
+        <v>43927</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>221</v>
+      </c>
+      <c r="B50" t="s">
+        <v>222</v>
+      </c>
+      <c r="C50" t="s">
+        <v>204</v>
+      </c>
+      <c r="D50" t="s">
+        <v>62</v>
+      </c>
+      <c r="E50" t="s">
+        <v>213</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="G50" s="4">
+        <v>43927</v>
+      </c>
+      <c r="H50" s="4">
+        <v>43927</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>226</v>
+      </c>
+      <c r="B51" t="s">
+        <v>227</v>
+      </c>
+      <c r="C51" t="s">
+        <v>204</v>
+      </c>
+      <c r="D51" t="s">
+        <v>212</v>
+      </c>
+      <c r="E51" t="s">
+        <v>228</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="G51" s="4">
+        <v>43927</v>
+      </c>
+      <c r="H51" s="4">
+        <v>43927</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>224</v>
+      </c>
+      <c r="B52" t="s">
+        <v>225</v>
+      </c>
+      <c r="C52" t="s">
+        <v>204</v>
+      </c>
+      <c r="D52" t="s">
+        <v>205</v>
+      </c>
+      <c r="E52" t="s">
+        <v>228</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="G52" s="4">
+        <v>43927</v>
+      </c>
+      <c r="H52" s="4">
+        <v>43927</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="B53" t="s">
+        <v>232</v>
+      </c>
+      <c r="C53" t="s">
+        <v>233</v>
+      </c>
+      <c r="D53" t="s">
+        <v>62</v>
+      </c>
+      <c r="E53" t="s">
+        <v>234</v>
+      </c>
+      <c r="G53" s="4">
+        <v>43928</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>235</v>
+      </c>
+      <c r="B54" s="13" t="s">
+        <v>236</v>
+      </c>
+      <c r="C54" t="s">
+        <v>237</v>
+      </c>
+      <c r="D54" t="s">
+        <v>238</v>
+      </c>
+      <c r="E54" t="s">
+        <v>234</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="G54" s="4">
+        <v>43929</v>
+      </c>
+      <c r="H54" s="4">
+        <v>43930</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" ht="28.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="6" t="s">
+        <v>240</v>
+      </c>
+      <c r="B55" t="s">
+        <v>241</v>
+      </c>
+      <c r="C55" t="s">
+        <v>242</v>
+      </c>
+      <c r="D55" t="s">
+        <v>243</v>
+      </c>
+      <c r="E55" t="s">
+        <v>244</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="G55" s="4">
+        <v>43930</v>
+      </c>
+      <c r="H55" s="4">
+        <v>43930</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="55.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>245</v>
+      </c>
+      <c r="B56" s="14" t="s">
+        <v>246</v>
+      </c>
+      <c r="C56" t="s">
+        <v>242</v>
+      </c>
+      <c r="D56" t="s">
+        <v>62</v>
+      </c>
+      <c r="E56" t="s">
+        <v>244</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="G56" s="4">
+        <v>43930</v>
+      </c>
+      <c r="H56" s="4">
+        <v>43931</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="B57" s="15" t="s">
+        <v>251</v>
+      </c>
+      <c r="C57" t="s">
+        <v>252</v>
+      </c>
+      <c r="D57" t="s">
+        <v>243</v>
+      </c>
+      <c r="E57" t="s">
+        <v>271</v>
+      </c>
+      <c r="G57" s="4">
+        <v>43930</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="96.6" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>253</v>
+      </c>
+      <c r="B58" t="s">
+        <v>254</v>
+      </c>
+      <c r="C58" t="s">
+        <v>242</v>
+      </c>
+      <c r="D58" t="s">
+        <v>243</v>
+      </c>
+      <c r="E58" t="s">
+        <v>271</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="G58" s="4">
+        <v>43931</v>
+      </c>
+      <c r="H58" s="4">
+        <v>43931</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="B59" t="s">
+        <v>257</v>
+      </c>
+      <c r="C59" t="s">
+        <v>242</v>
+      </c>
+      <c r="D59" t="s">
+        <v>243</v>
+      </c>
+      <c r="E59" t="s">
+        <v>268</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="G59" s="4">
+        <v>43931</v>
+      </c>
+      <c r="H59" s="4">
+        <v>43931</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>259</v>
+      </c>
+      <c r="B60" t="s">
+        <v>260</v>
+      </c>
+      <c r="C60" t="s">
+        <v>261</v>
+      </c>
+      <c r="D60" t="s">
+        <v>262</v>
+      </c>
+      <c r="E60" t="s">
+        <v>263</v>
+      </c>
+      <c r="G60" s="4">
+        <v>43934</v>
+      </c>
+      <c r="H60" s="4">
+        <v>43934</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>264</v>
+      </c>
+      <c r="B61" t="s">
+        <v>265</v>
+      </c>
+      <c r="C61" t="s">
+        <v>261</v>
+      </c>
+      <c r="D61" t="s">
+        <v>266</v>
+      </c>
+      <c r="E61" t="s">
+        <v>271</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="G61" s="4">
+        <v>43934</v>
+      </c>
+      <c r="H61" s="4">
+        <v>43934</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>274</v>
+      </c>
+      <c r="B62" t="s">
+        <v>275</v>
+      </c>
+      <c r="C62" t="s">
+        <v>261</v>
+      </c>
+      <c r="D62" t="s">
+        <v>266</v>
+      </c>
+      <c r="E62" t="s">
+        <v>276</v>
+      </c>
+      <c r="F62" s="16" t="s">
+        <v>277</v>
+      </c>
+      <c r="G62" s="4">
+        <v>43934</v>
+      </c>
+      <c r="H62" s="4">
+        <v>43934</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:H15" xr:uid="{880B8996-DDC7-47AA-9C04-AA5D01911FE9}"/>
+  <autoFilter ref="A1:H43" xr:uid="{880B8996-DDC7-47AA-9C04-AA5D01911FE9}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>